<commit_message>
Started 'points for' plot, some HTML, and starting to add d3js
</commit_message>
<xml_diff>
--- a/NapoliBallersHistory.xlsx
+++ b/NapoliBallersHistory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\R\NapoliBallers\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="37">
   <si>
     <t>Tom Gardner</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>Hans Biebl</t>
+  </si>
+  <si>
+    <t>draftOrder</t>
+  </si>
+  <si>
+    <t>Maksudul Ali</t>
+  </si>
+  <si>
+    <t>John Ross</t>
+  </si>
+  <si>
+    <t>winnings</t>
   </si>
 </sst>
 </file>
@@ -440,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K75"/>
+  <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="M66" sqref="M66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,9 +463,10 @@
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -487,8 +500,14 @@
       <c r="K1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -523,7 +542,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2010</v>
       </c>
@@ -558,7 +577,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2010</v>
       </c>
@@ -593,7 +612,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2010</v>
       </c>
@@ -628,7 +647,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2010</v>
       </c>
@@ -663,7 +682,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2010</v>
       </c>
@@ -698,7 +717,7 @@
         <v>-1.8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2010</v>
       </c>
@@ -733,7 +752,7 @@
         <v>-3.3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2010</v>
       </c>
@@ -768,7 +787,7 @@
         <v>-3.3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2010</v>
       </c>
@@ -803,7 +822,7 @@
         <v>-22.2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2010</v>
       </c>
@@ -838,7 +857,7 @@
         <v>-14.6</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2011</v>
       </c>
@@ -873,7 +892,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2011</v>
       </c>
@@ -908,7 +927,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2011</v>
       </c>
@@ -943,7 +962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -978,7 +997,7 @@
         <v>15.8</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2011</v>
       </c>
@@ -2133,7 +2152,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2014</v>
       </c>
@@ -2168,7 +2187,7 @@
         <v>17.100000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2014</v>
       </c>
@@ -2203,7 +2222,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2014</v>
       </c>
@@ -2238,7 +2257,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2014</v>
       </c>
@@ -2273,7 +2292,7 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2014</v>
       </c>
@@ -2308,7 +2327,7 @@
         <v>-16.100000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2014</v>
       </c>
@@ -2343,7 +2362,7 @@
         <v>-41.5</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2014</v>
       </c>
@@ -2378,7 +2397,7 @@
         <v>7.1</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2015</v>
       </c>
@@ -2412,8 +2431,11 @@
       <c r="K56">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M56">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2015</v>
       </c>
@@ -2447,8 +2469,11 @@
       <c r="K57">
         <v>-0.8</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M57">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2015</v>
       </c>
@@ -2482,8 +2507,11 @@
       <c r="K58">
         <v>16.899999999999999</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M58">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2015</v>
       </c>
@@ -2518,7 +2546,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2015</v>
       </c>
@@ -2553,7 +2581,7 @@
         <v>-9.4</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2015</v>
       </c>
@@ -2588,7 +2616,7 @@
         <v>-4.0999999999999996</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2015</v>
       </c>
@@ -2622,8 +2650,11 @@
       <c r="K62">
         <v>-10.6</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M62">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2015</v>
       </c>
@@ -2657,8 +2688,11 @@
       <c r="K63">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M63">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2015</v>
       </c>
@@ -2692,8 +2726,11 @@
       <c r="K64">
         <v>-7.4</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M64">
+        <v>-75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2015</v>
       </c>
@@ -2727,8 +2764,11 @@
       <c r="K65">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M65">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2016</v>
       </c>
@@ -2762,8 +2802,11 @@
       <c r="K66">
         <v>18.8</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M66">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2016</v>
       </c>
@@ -2797,8 +2840,11 @@
       <c r="K67">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M67">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2016</v>
       </c>
@@ -2832,8 +2878,11 @@
       <c r="K68">
         <v>29.2</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M68">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2016</v>
       </c>
@@ -2868,7 +2917,7 @@
         <v>-1.5</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2016</v>
       </c>
@@ -2903,7 +2952,7 @@
         <v>-1.6</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2016</v>
       </c>
@@ -2938,7 +2987,7 @@
         <v>-2.2000000000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2016</v>
       </c>
@@ -2972,8 +3021,11 @@
       <c r="K72">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M72">
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2016</v>
       </c>
@@ -3007,8 +3059,11 @@
       <c r="K73">
         <v>-17.5</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M73">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2016</v>
       </c>
@@ -3042,8 +3097,11 @@
       <c r="K74">
         <v>-19.399999999999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M74">
+        <v>-75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2016</v>
       </c>
@@ -3076,6 +3134,141 @@
       </c>
       <c r="K75">
         <v>-11.9</v>
+      </c>
+      <c r="M75">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>2017</v>
+      </c>
+      <c r="C76" t="s">
+        <v>1</v>
+      </c>
+      <c r="L76">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>2017</v>
+      </c>
+      <c r="C77" t="s">
+        <v>31</v>
+      </c>
+      <c r="L77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>2017</v>
+      </c>
+      <c r="C78" t="s">
+        <v>2</v>
+      </c>
+      <c r="L78">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>2017</v>
+      </c>
+      <c r="C79" t="s">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>2017</v>
+      </c>
+      <c r="C80" t="s">
+        <v>20</v>
+      </c>
+      <c r="L80">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>2017</v>
+      </c>
+      <c r="C81" t="s">
+        <v>32</v>
+      </c>
+      <c r="L81">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>2017</v>
+      </c>
+      <c r="C82" t="s">
+        <v>9</v>
+      </c>
+      <c r="L82">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>2017</v>
+      </c>
+      <c r="C83" t="s">
+        <v>6</v>
+      </c>
+      <c r="L83">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>2017</v>
+      </c>
+      <c r="C84" t="s">
+        <v>3</v>
+      </c>
+      <c r="L84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>2017</v>
+      </c>
+      <c r="C85" t="s">
+        <v>22</v>
+      </c>
+      <c r="L85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>2017</v>
+      </c>
+      <c r="C86" t="s">
+        <v>34</v>
+      </c>
+      <c r="L86">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>2017</v>
+      </c>
+      <c r="C87" t="s">
+        <v>35</v>
+      </c>
+      <c r="L87">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>